<commit_message>
Update 2025 Mighty Mu Student Codes.xlsx
</commit_message>
<xml_diff>
--- a/extra teams/2025 Mighty Mu Student Codes.xlsx
+++ b/extra teams/2025 Mighty Mu Student Codes.xlsx
@@ -331,13 +331,13 @@
     <t>Keston Carrier</t>
   </si>
   <si>
+    <t>Benjamin Cartwright</t>
+  </si>
+  <si>
+    <t>Elena Wiszowaty</t>
+  </si>
+  <si>
     <t>Gabriel Kerkinni</t>
-  </si>
-  <si>
-    <t>Benjamin Cartwright</t>
-  </si>
-  <si>
-    <t>Elena Wiszowaty</t>
   </si>
   <si>
     <t>Jacob Ciupka</t>
@@ -28230,8 +28230,8 @@
         <v>81</v>
       </c>
       <c r="E4" s="33" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("IFERROR(FILTER($G$9:$G$100, $C$9:$C$100=D4), ""NONE SELECTED"")"),"100301823")</f>
-        <v>100301823</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFERROR(FILTER($G$9:$G$100, $C$9:$C$100=D4), ""NONE SELECTED"")"),"100301522")</f>
+        <v>100301522</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="31"/>
@@ -28634,7 +28634,7 @@
       <c r="A23" s="43"/>
       <c r="B23" s="44"/>
       <c r="C23" s="45" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D23" s="46" t="str">
         <f t="shared" si="1"/>
@@ -28657,7 +28657,7 @@
       <c r="A24" s="56"/>
       <c r="B24" s="57"/>
       <c r="C24" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="59" t="str">
         <f t="shared" si="1"/>
@@ -28682,7 +28682,7 @@
       </c>
       <c r="B25" s="66"/>
       <c r="C25" s="91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" s="68" t="str">
         <f t="shared" si="1"/>
@@ -28704,7 +28704,7 @@
       </c>
       <c r="B26" s="72"/>
       <c r="C26" s="83" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="D26" s="74" t="str">
         <f t="shared" si="1"/>

</xml_diff>